<commit_message>
Some Updates Git Soap Katalon
</commit_message>
<xml_diff>
--- a/SoapUI/REST_API_Testing/TestData_CreateCustomers.xlsx
+++ b/SoapUI/REST_API_Testing/TestData_CreateCustomers.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\udemy\udemy_doku\SoapUI\REST_API_Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3DA8D6-E682-443D-940B-CA5355FF2CFC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6682D301-FCFD-421C-808A-595FC3422438}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13152" yWindow="3528" windowWidth="17280" windowHeight="8964" xr2:uid="{F6FA74FB-0357-4ED2-8C06-2397988B6C3A}"/>
+    <workbookView xWindow="1152" yWindow="3360" windowWidth="20220" windowHeight="8964" xr2:uid="{F6FA74FB-0357-4ED2-8C06-2397988B6C3A}"/>
   </bookViews>
   <sheets>
     <sheet name="customers" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="79">
   <si>
     <t>firstName</t>
   </si>
@@ -205,12 +205,76 @@
   </si>
   <si>
     <t>name9</t>
+  </si>
+  <si>
+    <t>created_customer_id</t>
+  </si>
+  <si>
+    <t>creation_date</t>
+  </si>
+  <si>
+    <t>cust7417744</t>
+  </si>
+  <si>
+    <t>Jun 24, 2019</t>
+  </si>
+  <si>
+    <t>cust8450268</t>
+  </si>
+  <si>
+    <t>cust5058747</t>
+  </si>
+  <si>
+    <t>cust4766501</t>
+  </si>
+  <si>
+    <t>cust4171411</t>
+  </si>
+  <si>
+    <t>cust7441665</t>
+  </si>
+  <si>
+    <t>cust8794934</t>
+  </si>
+  <si>
+    <t>cust8213313</t>
+  </si>
+  <si>
+    <t>cust8376131</t>
+  </si>
+  <si>
+    <t>cust8388157</t>
+  </si>
+  <si>
+    <t>cust7914541</t>
+  </si>
+  <si>
+    <t>cust2523276</t>
+  </si>
+  <si>
+    <t>cust3015161</t>
+  </si>
+  <si>
+    <t>cust5651821</t>
+  </si>
+  <si>
+    <t>cust7775609</t>
+  </si>
+  <si>
+    <t>cust5575266</t>
+  </si>
+  <si>
+    <t>cust3817227</t>
+  </si>
+  <si>
+    <t>cust7300786</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -236,12 +300,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -257,10 +333,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -576,47 +653,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB24CC4-E7FA-4262-9827-E5BD83057E4C}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="25.5546875" customWidth="1"/>
+    <col min="4" max="4" customWidth="true" width="25.5546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="18.88671875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.21875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -626,7 +711,7 @@
       <c r="C2">
         <v>27000</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E2" t="s">
@@ -644,8 +729,14 @@
       <c r="I2" t="s">
         <v>45</v>
       </c>
+      <c r="J2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -655,7 +746,7 @@
       <c r="C3">
         <v>27001</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E3" t="s">
@@ -673,8 +764,14 @@
       <c r="I3" t="s">
         <v>45</v>
       </c>
+      <c r="J3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -684,7 +781,7 @@
       <c r="C4">
         <v>27002</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E4" t="s">
@@ -702,8 +799,14 @@
       <c r="I4" t="s">
         <v>46</v>
       </c>
+      <c r="J4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -713,7 +816,7 @@
       <c r="C5">
         <v>27003</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E5" t="s">
@@ -731,8 +834,14 @@
       <c r="I5" t="s">
         <v>47</v>
       </c>
+      <c r="J5" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -742,7 +851,7 @@
       <c r="C6">
         <v>27004</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E6" t="s">
@@ -760,8 +869,14 @@
       <c r="I6" t="s">
         <v>45</v>
       </c>
+      <c r="J6" t="s">
+        <v>74</v>
+      </c>
+      <c r="K6" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -771,7 +886,7 @@
       <c r="C7">
         <v>27005</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E7" t="s">
@@ -789,8 +904,14 @@
       <c r="I7" t="s">
         <v>45</v>
       </c>
+      <c r="J7" t="s">
+        <v>75</v>
+      </c>
+      <c r="K7" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -800,7 +921,7 @@
       <c r="C8">
         <v>27006</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E8" t="s">
@@ -818,8 +939,14 @@
       <c r="I8" t="s">
         <v>45</v>
       </c>
+      <c r="J8" t="s">
+        <v>76</v>
+      </c>
+      <c r="K8" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -829,7 +956,7 @@
       <c r="C9">
         <v>27007</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E9" t="s">
@@ -847,8 +974,14 @@
       <c r="I9" t="s">
         <v>48</v>
       </c>
+      <c r="J9" t="s">
+        <v>77</v>
+      </c>
+      <c r="K9" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -858,7 +991,7 @@
       <c r="C10">
         <v>27008</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E10" t="s">
@@ -875,6 +1008,12 @@
       </c>
       <c r="I10" t="s">
         <v>48</v>
+      </c>
+      <c r="J10" t="s">
+        <v>78</v>
+      </c>
+      <c r="K10" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>